<commit_message>
Agregando archivos actualizados del proyecto
</commit_message>
<xml_diff>
--- a/Documentos/Entrega 4/Cronograma.xlsx
+++ b/Documentos/Entrega 4/Cronograma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\OneDrive\Documents\Equipo-1-05_02\Documentos\Entrega 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38CA2E9-CA46-4DE3-8E8F-41946BC1B9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5AA052-D898-45C2-8451-C352ACBF75E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3210" windowWidth="18900" windowHeight="11055" activeTab="1" xr2:uid="{194D59EC-A3A2-47E8-8329-7C73CE427850}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{194D59EC-A3A2-47E8-8329-7C73CE427850}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>Etapa 4</t>
   </si>
   <si>
-    <t>Etapa 6</t>
-  </si>
-  <si>
     <t>Entrega Finalizada</t>
   </si>
   <si>
@@ -206,6 +203,9 @@
   </si>
   <si>
     <t>HU13: Gestión de Secadoras</t>
+  </si>
+  <si>
+    <t>Etapa 5</t>
   </si>
 </sst>
 </file>
@@ -791,6 +791,7 @@
     <xf numFmtId="9" fontId="10" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="10" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -862,7 +863,6 @@
     <xf numFmtId="165" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Énfasis1" xfId="2" builtinId="30"/>
@@ -1079,6 +1079,10 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="36" fmlaLink="$E$32" max="30" min="1" page="10"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp44.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="36" fmlaLink="$E$31" max="30" min="1" page="10"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="36" fmlaLink="$F$12" max="30" page="10" val="7"/>
 </file>
@@ -3256,13 +3260,63 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>19050</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>295275</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>247650</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2131" name="Spinner 83" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2131"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000053080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3300,7 +3354,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3406,7 +3460,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3548,7 +3602,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3575,36 +3629,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
-      <c r="AE1" s="72"/>
-      <c r="AF1" s="72"/>
-      <c r="AG1" s="72"/>
-      <c r="AH1" s="72"/>
-      <c r="AI1" s="72"/>
-      <c r="AJ1" s="72"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
+      <c r="AB1" s="73"/>
+      <c r="AC1" s="73"/>
+      <c r="AD1" s="73"/>
+      <c r="AE1" s="73"/>
+      <c r="AF1" s="73"/>
+      <c r="AG1" s="73"/>
+      <c r="AH1" s="73"/>
+      <c r="AI1" s="73"/>
+      <c r="AJ1" s="73"/>
     </row>
     <row r="2" spans="1:36" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I2" s="16"/>
@@ -3613,67 +3667,67 @@
       <c r="L2" s="16">
         <v>0</v>
       </c>
-      <c r="M2" s="80">
+      <c r="M2" s="81">
         <f>E4+L2</f>
         <v>44470</v>
       </c>
-      <c r="N2" s="80"/>
+      <c r="N2" s="81"/>
     </row>
     <row r="3" spans="1:36" ht="20.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I3" s="81">
+      <c r="I3" s="82">
         <f>I4</f>
         <v>44470</v>
       </c>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="84">
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="85">
         <f t="shared" ref="P3" si="0">P4</f>
         <v>44477</v>
       </c>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="85"/>
-      <c r="V3" s="86"/>
-      <c r="W3" s="81">
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="82">
         <f t="shared" ref="W3" si="1">W4</f>
         <v>44484</v>
       </c>
-      <c r="X3" s="82"/>
-      <c r="Y3" s="82"/>
-      <c r="Z3" s="82"/>
-      <c r="AA3" s="82"/>
-      <c r="AB3" s="82"/>
-      <c r="AC3" s="83"/>
-      <c r="AD3" s="84">
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="83"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="83"/>
+      <c r="AC3" s="84"/>
+      <c r="AD3" s="85">
         <f t="shared" ref="AD3" si="2">AD4</f>
         <v>44491</v>
       </c>
-      <c r="AE3" s="85"/>
-      <c r="AF3" s="85"/>
-      <c r="AG3" s="85"/>
-      <c r="AH3" s="85"/>
-      <c r="AI3" s="85"/>
-      <c r="AJ3" s="86"/>
+      <c r="AE3" s="86"/>
+      <c r="AF3" s="86"/>
+      <c r="AG3" s="86"/>
+      <c r="AH3" s="86"/>
+      <c r="AI3" s="86"/>
+      <c r="AJ3" s="87"/>
     </row>
     <row r="4" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="75">
+      <c r="E4" s="76">
         <v>44470</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="78"/>
       <c r="I4" s="10">
         <f>M2</f>
         <v>44470</v>
@@ -3804,10 +3858,10 @@
       <c r="F5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="74"/>
+      <c r="H5" s="75"/>
       <c r="I5" s="11" t="str">
         <f>TEXT(I4,"ddd")</f>
         <v>vie</v>
@@ -5017,8 +5071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3644728F-21C7-47C3-AAD3-1E6CBD0ADAEB}">
   <dimension ref="A2:AX287"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AM7" sqref="AM7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5047,58 +5101,58 @@
     </row>
     <row r="3" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G3" s="26"/>
-      <c r="H3" s="96">
+      <c r="H3" s="97">
         <f>H4</f>
         <v>45720</v>
       </c>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="87">
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="88">
         <f t="shared" ref="O3" si="0">O4</f>
         <v>45727</v>
       </c>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="87"/>
-      <c r="S3" s="87"/>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="96">
+      <c r="P3" s="88"/>
+      <c r="Q3" s="88"/>
+      <c r="R3" s="88"/>
+      <c r="S3" s="88"/>
+      <c r="T3" s="88"/>
+      <c r="U3" s="88"/>
+      <c r="V3" s="97">
         <f t="shared" ref="V3" si="1">V4</f>
         <v>45734</v>
       </c>
-      <c r="W3" s="96"/>
-      <c r="X3" s="96"/>
-      <c r="Y3" s="96"/>
-      <c r="Z3" s="96"/>
-      <c r="AA3" s="96"/>
-      <c r="AB3" s="96"/>
-      <c r="AC3" s="87">
+      <c r="W3" s="97"/>
+      <c r="X3" s="97"/>
+      <c r="Y3" s="97"/>
+      <c r="Z3" s="97"/>
+      <c r="AA3" s="97"/>
+      <c r="AB3" s="97"/>
+      <c r="AC3" s="88">
         <f t="shared" ref="AC3" si="2">AC4</f>
         <v>45741</v>
       </c>
-      <c r="AD3" s="87"/>
-      <c r="AE3" s="87"/>
-      <c r="AF3" s="87"/>
-      <c r="AG3" s="87"/>
-      <c r="AH3" s="87"/>
-      <c r="AI3" s="87"/>
+      <c r="AD3" s="88"/>
+      <c r="AE3" s="88"/>
+      <c r="AF3" s="88"/>
+      <c r="AG3" s="88"/>
+      <c r="AH3" s="88"/>
+      <c r="AI3" s="88"/>
     </row>
     <row r="4" spans="1:50" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="88">
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="89">
         <v>45720</v>
       </c>
-      <c r="E4" s="88"/>
-      <c r="F4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="90"/>
       <c r="G4" s="65"/>
       <c r="H4" s="27">
         <f>I2</f>
@@ -5244,10 +5298,10 @@
       <c r="E5" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="94" t="s">
+      <c r="F5" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="95"/>
+      <c r="G5" s="96"/>
       <c r="H5" s="28" t="str">
         <f>TEXT(H4,"ddd")</f>
         <v>mar</v>
@@ -5608,17 +5662,17 @@
         <v>35</v>
       </c>
       <c r="C11" s="35">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D11" s="36">
         <v>45721</v>
       </c>
       <c r="E11" s="37">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F11" s="36">
-        <f t="shared" si="5"/>
-        <v>45758</v>
+        <f>D11+E11-1</f>
+        <v>45759</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="29"/>
@@ -5657,7 +5711,7 @@
       <c r="B12" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="97">
+      <c r="C12" s="72">
         <v>1</v>
       </c>
       <c r="D12" s="36">
@@ -5791,7 +5845,7 @@
     </row>
     <row r="15" spans="1:50" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="67" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="39" t="s">
         <v>34</v>
@@ -5841,7 +5895,7 @@
     </row>
     <row r="16" spans="1:50" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="67" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="39" t="s">
         <v>35</v>
@@ -5891,7 +5945,7 @@
     </row>
     <row r="17" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="67" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="39" t="s">
         <v>34</v>
@@ -5941,7 +5995,7 @@
     </row>
     <row r="18" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="39" t="s">
         <v>33</v>
@@ -5991,7 +6045,7 @@
     </row>
     <row r="19" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="39" t="s">
         <v>34</v>
@@ -6041,7 +6095,7 @@
     </row>
     <row r="20" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="39" t="s">
         <v>33</v>
@@ -6091,7 +6145,7 @@
     </row>
     <row r="21" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="39" t="s">
         <v>33</v>
@@ -6180,7 +6234,7 @@
     </row>
     <row r="23" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="68" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="44" t="s">
         <v>34</v>
@@ -6230,7 +6284,7 @@
     </row>
     <row r="24" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="44" t="s">
         <v>33</v>
@@ -6280,7 +6334,7 @@
     </row>
     <row r="25" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="66" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="44" t="s">
         <v>34</v>
@@ -6330,7 +6384,7 @@
     </row>
     <row r="26" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" s="44" t="s">
         <v>33</v>
@@ -6419,7 +6473,7 @@
     </row>
     <row r="28" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="49" t="s">
         <v>34</v>
@@ -6469,7 +6523,7 @@
     </row>
     <row r="29" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="49" t="s">
         <v>33</v>
@@ -6519,7 +6573,7 @@
     </row>
     <row r="30" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="53" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B30" s="54"/>
       <c r="C30" s="55"/>
@@ -6558,17 +6612,24 @@
     </row>
     <row r="31" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31" s="54" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="55">
-        <v>0</v>
-      </c>
-      <c r="D31" s="56"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="56"/>
+        <v>1</v>
+      </c>
+      <c r="D31" s="56">
+        <v>45759</v>
+      </c>
+      <c r="E31" s="57">
+        <v>1</v>
+      </c>
+      <c r="F31" s="56">
+        <f>D31+E31-1</f>
+        <v>45759</v>
+      </c>
       <c r="G31" s="54"/>
       <c r="H31" s="29"/>
       <c r="I31" s="29"/>
@@ -6601,23 +6662,23 @@
     </row>
     <row r="32" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="54" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="56">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="E32" s="57">
         <v>1</v>
       </c>
       <c r="F32" s="56">
-        <f t="shared" si="8"/>
-        <v>45754</v>
+        <f>D32+E32-1</f>
+        <v>45759</v>
       </c>
       <c r="G32" s="54"/>
       <c r="H32" s="29"/>
@@ -6651,23 +6712,23 @@
     </row>
     <row r="33" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" s="54" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="56">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="E33" s="57">
         <v>1</v>
       </c>
       <c r="F33" s="56">
         <f t="shared" si="8"/>
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="G33" s="54"/>
       <c r="H33" s="29"/>
@@ -6701,16 +6762,16 @@
     </row>
     <row r="34" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="60"/>
-      <c r="C34" s="92">
-        <v>45760</v>
-      </c>
-      <c r="D34" s="92"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="92"/>
-      <c r="G34" s="93"/>
+      <c r="C34" s="93">
+        <v>45763</v>
+      </c>
+      <c r="D34" s="93"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="94"/>
       <c r="H34" s="29"/>
       <c r="I34" s="29"/>
       <c r="J34" s="29"/>
@@ -6757,16 +6818,6 @@
     <mergeCell ref="V3:AB3"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="H7:AI33">
-    <cfRule type="expression" dxfId="2" priority="17">
-      <formula>AND(H$4&gt;=$D7,H$4&lt;=$F7)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7:AI34">
-    <cfRule type="expression" dxfId="1" priority="12">
-      <formula>"Y(H$4&gt;=$D7;H$4&lt;=$F7)"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C27">
     <cfRule type="dataBar" priority="4">
       <dataBar>
@@ -6795,11 +6846,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34:AI34">
-    <cfRule type="expression" dxfId="0" priority="23">
-      <formula>AND(H$4&gt;=$C34,H$4&lt;=$F34)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C31:C33 C7:C26 C28:C29">
     <cfRule type="dataBar" priority="30">
       <dataBar>
@@ -6812,6 +6858,21 @@
           <x14:id>{FC4D732F-7040-4173-9471-66C86A405DB9}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:AI33">
+    <cfRule type="expression" dxfId="2" priority="17">
+      <formula>AND(H$4&gt;=$D7,H$4&lt;=$F7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:AI34">
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>"Y(H$4&gt;=$D7;H$4&lt;=$F7)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:AI34">
+    <cfRule type="expression" dxfId="0" priority="23">
+      <formula>AND(H$4&gt;=$C34,H$4&lt;=$F34)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7481,6 +7542,28 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2131" r:id="rId34" name="Spinner 83">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:row>30</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>295275</xdr:colOff>
+                    <xdr:row>30</xdr:row>
+                    <xdr:rowOff>247650</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>